<commit_message>
Add Shift Register to ALU
+ added control logic to shift reg
</commit_message>
<xml_diff>
--- a/8Bit Computer ver2.0/excel/commands.xlsx
+++ b/8Bit Computer ver2.0/excel/commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Github Repo\Computer_HTL\8Bit Computer ver2.0\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F384469D-60E7-4F94-9177-6E426361751D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC6F9BA-FA69-4135-8E42-A85C936D2AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40365" yWindow="3090" windowWidth="28800" windowHeight="15345" xr2:uid="{3256ACAE-F419-450F-8F49-2183F1DCCADE}"/>
+    <workbookView xWindow="4665" yWindow="3480" windowWidth="28800" windowHeight="15345" xr2:uid="{3256ACAE-F419-450F-8F49-2183F1DCCADE}"/>
   </bookViews>
   <sheets>
     <sheet name="Commands" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="82">
   <si>
     <t>NOP</t>
   </si>
@@ -55,12 +55,6 @@
     <t>LOAD FLAGS</t>
   </si>
   <si>
-    <t>SHIFT LEFT</t>
-  </si>
-  <si>
-    <t>LOAD SHIFT REG</t>
-  </si>
-  <si>
     <t>OTHER</t>
   </si>
   <si>
@@ -70,9 +64,6 @@
     <t>CLEAR B</t>
   </si>
   <si>
-    <t>CLEAR SHIFT REG</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -103,9 +94,6 @@
     <t>&gt; would add one more step to most calculations, but is the simplest solution</t>
   </si>
   <si>
-    <t>SHIFT RIGHT</t>
-  </si>
-  <si>
     <t>FLAG REGISTER</t>
   </si>
   <si>
@@ -278,6 +266,12 @@
   </si>
   <si>
     <t>STORE B</t>
+  </si>
+  <si>
+    <t>SHIFT</t>
+  </si>
+  <si>
+    <t>SHIFT CIRCULAR</t>
   </si>
 </sst>
 </file>
@@ -796,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02BDFC33-BE10-4835-94A0-E5C8BC037442}">
-  <dimension ref="A1:P56"/>
+  <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,45 +812,45 @@
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C1" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I1" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>57</v>
-      </c>
       <c r="N1" s="10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="2"/>
@@ -882,51 +876,51 @@
       <c r="C3" s="5"/>
       <c r="D3" s="6"/>
       <c r="E3" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="3"/>
       <c r="M3" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="N3" s="13"/>
       <c r="P3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="6"/>
       <c r="E4" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="N4" s="13"/>
     </row>
@@ -937,25 +931,25 @@
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>
       <c r="E5" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="3"/>
       <c r="M5" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="N5" s="13"/>
       <c r="P5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -972,12 +966,12 @@
       <c r="M6" s="4"/>
       <c r="N6" s="13"/>
       <c r="P6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>6</v>
@@ -987,17 +981,17 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="3"/>
       <c r="M7" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="N7" s="13"/>
     </row>
@@ -1010,21 +1004,21 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="3"/>
       <c r="M8" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="N8" s="13"/>
       <c r="P8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -1043,20 +1037,20 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="6"/>
@@ -1067,7 +1061,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
@@ -1101,18 +1095,18 @@
         <v>3</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
       <c r="E13" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
@@ -1122,20 +1116,20 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
       <c r="E14" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
@@ -1143,25 +1137,25 @@
       <c r="M14" s="4"/>
       <c r="N14" s="13"/>
       <c r="P14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
       <c r="E15" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
@@ -1169,25 +1163,25 @@
       <c r="M15" s="4"/>
       <c r="N15" s="13"/>
       <c r="P15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16" s="14" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
@@ -1195,23 +1189,23 @@
       <c r="M16" s="4"/>
       <c r="N16" s="13"/>
       <c r="P16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
       <c r="E17" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
@@ -1221,20 +1215,20 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B18" s="14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
       <c r="E18" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
@@ -1242,25 +1236,25 @@
       <c r="M18" s="4"/>
       <c r="N18" s="13"/>
       <c r="P18" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
       <c r="E19" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
@@ -1268,25 +1262,25 @@
       <c r="M19" s="4"/>
       <c r="N19" s="13"/>
       <c r="P19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B20" s="14" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
       <c r="E20" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
@@ -1313,76 +1307,76 @@
         <v>4</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
       <c r="E22" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
       <c r="L22" s="3"/>
       <c r="M22" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="N22" s="13"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B23" s="14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
       <c r="E23" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
       <c r="L23" s="3"/>
       <c r="M23" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="N23" s="13"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B24" s="14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
       <c r="E24" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
       <c r="L24" s="3"/>
       <c r="M24" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="N24" s="13"/>
     </row>
@@ -1402,20 +1396,20 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I26" s="3"/>
       <c r="J26" s="6"/>
@@ -1426,17 +1420,17 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="6"/>
@@ -1447,7 +1441,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="6"/>
@@ -1464,7 +1458,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
@@ -1481,7 +1475,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="6"/>
@@ -1512,7 +1506,7 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B32" t="s">
         <v>8</v>
@@ -1524,19 +1518,19 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
       <c r="L32" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="M32" s="4"/>
       <c r="N32" s="13"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="6"/>
@@ -1549,7 +1543,7 @@
       <c r="K33" s="6"/>
       <c r="L33" s="3"/>
       <c r="M33" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="N33" s="13"/>
     </row>
@@ -1569,20 +1563,22 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>27</v>
-      </c>
-      <c r="B35" t="s">
-        <v>10</v>
-      </c>
-      <c r="C35" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="D35" s="6"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
-      <c r="H35" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="J35" s="6"/>
       <c r="K35" s="6"/>
       <c r="L35" s="3"/>
@@ -1590,10 +1586,12 @@
       <c r="N35" s="13"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36" s="5"/>
+      <c r="B36" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="D36" s="6"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
@@ -1606,136 +1604,136 @@
       <c r="M36" s="4"/>
       <c r="N36" s="13"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>43</v>
-      </c>
+    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="5"/>
       <c r="D37" s="6"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
-      <c r="I37" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="I37" s="3"/>
       <c r="J37" s="6"/>
       <c r="K37" s="6"/>
       <c r="L37" s="3"/>
       <c r="M37" s="4"/>
-      <c r="N37" s="13"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D38" s="6"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="13"/>
-    </row>
-    <row r="39" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N37" s="4"/>
+    </row>
+    <row r="38" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="J38" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="K38" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="L38" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="M38" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="N38" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="18"/>
       <c r="C39" s="5"/>
       <c r="D39" s="6"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
-    </row>
-    <row r="40" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H40" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="I40" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="J40" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="K40" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="L40" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="M40" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="N40" s="10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="5"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
       <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
+      <c r="K41" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="L41" s="6"/>
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>46</v>
-      </c>
       <c r="B42" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="H42" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I42" s="6"/>
       <c r="J42" s="6"/>
       <c r="K42" s="6"/>
       <c r="L42" s="6"/>
@@ -1744,10 +1742,10 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="11"/>
@@ -1755,28 +1753,21 @@
       <c r="G43" s="11"/>
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
-      <c r="J43" s="6"/>
-      <c r="K43" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="J43" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K43" s="6"/>
       <c r="L43" s="6"/>
       <c r="M43" s="7"/>
       <c r="N43" s="7"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>49</v>
-      </c>
       <c r="C44" s="5"/>
-      <c r="D44" s="6" t="s">
-        <v>42</v>
-      </c>
+      <c r="D44" s="6"/>
       <c r="E44" s="11"/>
       <c r="F44" s="11"/>
       <c r="G44" s="11"/>
-      <c r="H44" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="H44" s="6"/>
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
       <c r="K44" s="6"/>
@@ -1785,33 +1776,41 @@
       <c r="N44" s="7"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>62</v>
+      </c>
       <c r="B45" t="s">
-        <v>50</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>42</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C45" s="5"/>
       <c r="D45" s="6"/>
       <c r="E45" s="11"/>
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
       <c r="H45" s="6"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="I45" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J45" s="6"/>
       <c r="K45" s="6"/>
       <c r="L45" s="6"/>
       <c r="M45" s="7"/>
       <c r="N45" s="7"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C46" s="5"/>
+      <c r="B46" t="s">
+        <v>45</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D46" s="6"/>
       <c r="E46" s="11"/>
       <c r="F46" s="11"/>
       <c r="G46" s="11"/>
-      <c r="H46" s="6"/>
+      <c r="H46" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
       <c r="K46" s="6"/>
@@ -1820,11 +1819,8 @@
       <c r="N46" s="7"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>66</v>
-      </c>
       <c r="B47" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="6"/>
@@ -1832,9 +1828,7 @@
       <c r="F47" s="11"/>
       <c r="G47" s="11"/>
       <c r="H47" s="6"/>
-      <c r="I47" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="I47" s="6"/>
       <c r="J47" s="6"/>
       <c r="K47" s="6"/>
       <c r="L47" s="6"/>
@@ -1843,18 +1837,14 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>49</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>41</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C48" s="5"/>
       <c r="D48" s="6"/>
       <c r="E48" s="11"/>
       <c r="F48" s="11"/>
       <c r="G48" s="11"/>
-      <c r="H48" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="H48" s="6"/>
       <c r="I48" s="6"/>
       <c r="J48" s="6"/>
       <c r="K48" s="6"/>
@@ -1864,7 +1854,7 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="6"/>
@@ -1897,9 +1887,6 @@
       <c r="N50" s="7"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>70</v>
-      </c>
       <c r="C51" s="5"/>
       <c r="D51" s="6"/>
       <c r="E51" s="11"/>
@@ -1914,108 +1901,77 @@
       <c r="N51" s="7"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>9</v>
+      </c>
       <c r="B52" t="s">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="6"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="6"/>
-      <c r="I52" s="6"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="12"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
-      <c r="L52" s="6"/>
-      <c r="M52" s="7"/>
-      <c r="N52" s="7"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="4"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>70</v>
+      </c>
       <c r="C53" s="5"/>
-      <c r="D53" s="6"/>
+      <c r="D53" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="E53" s="11"/>
       <c r="F53" s="11"/>
       <c r="G53" s="11"/>
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
-      <c r="J53" s="6"/>
+      <c r="J53" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="K53" s="6"/>
       <c r="L53" s="6"/>
       <c r="M53" s="7"/>
-      <c r="N53" s="7"/>
+      <c r="N53" s="7" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>11</v>
-      </c>
       <c r="B54" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="C54" s="5"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
-      <c r="J54" s="6"/>
+      <c r="D54" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I54" s="6"/>
+      <c r="J54" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="K54" s="6"/>
-      <c r="L54" s="3"/>
-      <c r="M54" s="4"/>
-      <c r="N54" s="4"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>74</v>
-      </c>
-      <c r="C55" s="5"/>
-      <c r="D55" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="6"/>
-      <c r="I55" s="6"/>
-      <c r="J55" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K55" s="6"/>
-      <c r="L55" s="6"/>
-      <c r="M55" s="7"/>
-      <c r="N55" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>73</v>
-      </c>
-      <c r="C56" s="5"/>
-      <c r="D56" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E56" s="11"/>
-      <c r="F56" s="11"/>
-      <c r="G56" s="11"/>
-      <c r="H56" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I56" s="6"/>
-      <c r="J56" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K56" s="6"/>
-      <c r="L56" s="6"/>
-      <c r="M56" s="7"/>
-      <c r="N56" s="7" t="s">
-        <v>15</v>
+      <c r="L54" s="6"/>
+      <c r="M54" s="7"/>
+      <c r="N54" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A39:B39"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2039,7 +1995,7 @@
   <sheetData>
     <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B2" s="16"/>
     </row>
@@ -2048,62 +2004,62 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B13" s="16"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started work on 8 to 16 bit converter
</commit_message>
<xml_diff>
--- a/8Bit Computer ver2.0/excel/commands.xlsx
+++ b/8Bit Computer ver2.0/excel/commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\GitHub\Private\Computer_HTL\8Bit Computer ver2.0\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC9549E-2E11-4017-BF7F-975735A8A956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB90E070-4FE8-4563-8976-2AFC8FD2158B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3256ACAE-F419-450F-8F49-2183F1DCCADE}"/>
   </bookViews>
@@ -460,18 +460,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -484,6 +472,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -822,7 +822,7 @@
   <dimension ref="A1:P56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:XFD40"/>
+      <selection activeCell="T37" sqref="T37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,10 +878,10 @@
       </c>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="17"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="2"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -1635,43 +1635,43 @@
       <c r="A36" t="s">
         <v>21</v>
       </c>
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="C36" s="21" t="s">
+      <c r="C36" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D36" s="22"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="J36" s="22"/>
-      <c r="K36" s="22"/>
-      <c r="L36" s="23"/>
-      <c r="M36" s="24"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="20"/>
       <c r="N36" s="13"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="21" t="s">
+      <c r="C37" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="22"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="23"/>
-      <c r="J37" s="22"/>
-      <c r="K37" s="22"/>
-      <c r="L37" s="23"/>
-      <c r="M37" s="24"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="20"/>
       <c r="N37" s="13"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -1741,10 +1741,10 @@
       </c>
     </row>
     <row r="41" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="18" t="s">
+      <c r="A41" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B41" s="19"/>
+      <c r="B41" s="24"/>
       <c r="C41" s="5"/>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
@@ -1783,7 +1783,7 @@
       <c r="N42" s="7"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+      <c r="B43" s="15" t="s">
         <v>41</v>
       </c>
       <c r="C43" s="5" t="s">
@@ -1825,7 +1825,7 @@
       <c r="N44" s="7"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+      <c r="B45" s="15" t="s">
         <v>43</v>
       </c>
       <c r="C45" s="5" t="s">
@@ -2078,10 +2078,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="17"/>
+      <c r="B2" s="22"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2128,10 +2128,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="17"/>
+      <c r="B13" s="22"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">

</xml_diff>

<commit_message>
finished the 8 to 16 converter
</commit_message>
<xml_diff>
--- a/8Bit Computer ver2.0/excel/commands.xlsx
+++ b/8Bit Computer ver2.0/excel/commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\GitHub\Private\Computer_HTL\8Bit Computer ver2.0\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB90E070-4FE8-4563-8976-2AFC8FD2158B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44278C0-EA1B-493F-9313-C4B4735270D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3256ACAE-F419-450F-8F49-2183F1DCCADE}"/>
   </bookViews>
@@ -821,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02BDFC33-BE10-4835-94A0-E5C8BC037442}">
   <dimension ref="A1:P56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T37" sqref="T37"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S38" sqref="S38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1783,7 +1783,7 @@
       <c r="N42" s="7"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="14" t="s">
         <v>41</v>
       </c>
       <c r="C43" s="5" t="s">
@@ -1825,7 +1825,7 @@
       <c r="N44" s="7"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="14" t="s">
         <v>43</v>
       </c>
       <c r="C45" s="5" t="s">

</xml_diff>

<commit_message>
added 2 more commands
- LD to register 1
- LD to register 2
both together are one big 16 bit register for ram to be able to write to the full addr bus
</commit_message>
<xml_diff>
--- a/8Bit Computer ver2.0/excel/commands.xlsx
+++ b/8Bit Computer ver2.0/excel/commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\GitHub\Private\Computer_HTL\8Bit Computer ver2.0\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF419017-1126-4187-A82F-AD54AABD8E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D57577-23EB-44D6-9672-6211D62D7949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{3256ACAE-F419-450F-8F49-2183F1DCCADE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3256ACAE-F419-450F-8F49-2183F1DCCADE}"/>
   </bookViews>
   <sheets>
     <sheet name="Commands" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="131">
   <si>
     <t>NOP</t>
   </si>
@@ -407,6 +407,18 @@
   </si>
   <si>
     <t>0x25</t>
+  </si>
+  <si>
+    <t>LOAD to register 1 (for output to addr bus)</t>
+  </si>
+  <si>
+    <t>LOAD to register 2 (for output to addr bus)</t>
+  </si>
+  <si>
+    <t>0x26</t>
+  </si>
+  <si>
+    <t>0x27</t>
   </si>
 </sst>
 </file>
@@ -589,7 +601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -628,22 +640,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -652,13 +662,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -998,7 +1005,7 @@
   <dimension ref="A1:AH76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,47 +1026,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="24" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="L1" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="M1" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="N1" s="24" t="s">
+      <c r="N1" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="O1" s="25" t="s">
+      <c r="O1" s="20" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1070,7 +1077,7 @@
       <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="21" t="s">
         <v>89</v>
       </c>
       <c r="D2" s="4"/>
@@ -1090,7 +1097,7 @@
       <c r="B3" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="21" t="s">
         <v>90</v>
       </c>
       <c r="D3" s="4"/>
@@ -1119,7 +1126,7 @@
       <c r="B4" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="21" t="s">
         <v>91</v>
       </c>
       <c r="D4" s="4"/>
@@ -1147,10 +1154,10 @@
       <c r="A5" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="21" t="s">
         <v>92</v>
       </c>
       <c r="D5" s="4"/>
@@ -1172,11 +1179,10 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="21" t="s">
         <v>93</v>
       </c>
       <c r="D6" s="4"/>
@@ -1198,10 +1204,10 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="21" t="s">
         <v>94</v>
       </c>
       <c r="D7" s="4"/>
@@ -1222,10 +1228,10 @@
       <c r="O7" s="6"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="21" t="s">
         <v>95</v>
       </c>
       <c r="D8" s="4"/>
@@ -1249,7 +1255,7 @@
       <c r="B9" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="21" t="s">
         <v>96</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -1276,7 +1282,7 @@
       <c r="B10" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -1296,141 +1302,123 @@
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
     </row>
-    <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" s="21" t="s">
         <v>98</v>
       </c>
       <c r="D11" s="4"/>
-      <c r="E11" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="E11" s="5"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
-      <c r="L11" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="L11" s="5"/>
       <c r="M11" s="5"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
     </row>
-    <row r="12" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="28" t="s">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+    </row>
+    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M13" s="5"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+    </row>
+    <row r="14" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="24" t="s">
+      <c r="B14" s="23"/>
+      <c r="C14" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D14" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E14" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="24" t="s">
+      <c r="F14" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="24" t="s">
+      <c r="G14" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="H14" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="I12" s="24" t="s">
+      <c r="I14" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="J12" s="24" t="s">
+      <c r="J14" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="K12" s="24" t="s">
+      <c r="K14" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="L12" s="24" t="s">
+      <c r="L14" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="M12" s="24" t="s">
+      <c r="M14" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="N12" s="24" t="s">
+      <c r="N14" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="O12" s="25" t="s">
+      <c r="O14" s="20" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B15" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="O13" s="9"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="O14" s="9"/>
-    </row>
-    <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="21" t="s">
         <v>101</v>
       </c>
       <c r="D15" s="4"/>
@@ -1455,51 +1443,54 @@
       <c r="O15" s="9"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="30" t="s">
+      <c r="B16" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="21" t="s">
         <v>102</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="F16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
-      <c r="M16" s="2"/>
+      <c r="M16" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="N16" s="3" t="s">
         <v>10</v>
       </c>
       <c r="O16" s="9"/>
     </row>
-    <row r="17" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="30" t="s">
+    <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="21" t="s">
         <v>103</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="F17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
@@ -1508,45 +1499,41 @@
         <v>10</v>
       </c>
       <c r="O17" s="9"/>
-      <c r="Q17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>34</v>
-      </c>
+      <c r="D18" s="4"/>
       <c r="E18" s="5"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J18" s="2"/>
+      <c r="H18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="2"/>
-      <c r="N18" s="3"/>
+      <c r="N18" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="O18" s="9"/>
-      <c r="Q18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="30" t="s">
+    </row>
+    <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="21" t="s">
         <v>105</v>
       </c>
       <c r="D19" s="4"/>
@@ -1558,60 +1545,63 @@
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="2"/>
-      <c r="N19" s="3"/>
+      <c r="N19" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="O19" s="9"/>
       <c r="Q19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="4"/>
+      <c r="D20" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="E20" s="5"/>
-      <c r="F20" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="I20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" s="2"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="2"/>
       <c r="N20" s="3"/>
       <c r="O20" s="9"/>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="21" t="s">
         <v>107</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="5"/>
-      <c r="F21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2" t="s">
         <v>10</v>
@@ -1622,14 +1612,17 @@
       <c r="N21" s="3"/>
       <c r="O21" s="9"/>
       <c r="Q21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="21" t="s">
         <v>108</v>
       </c>
       <c r="D22" s="4"/>
@@ -1637,9 +1630,7 @@
       <c r="F22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2" t="s">
@@ -1650,15 +1641,12 @@
       <c r="M22" s="2"/>
       <c r="N22" s="3"/>
       <c r="O22" s="9"/>
-      <c r="Q22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="21" t="s">
         <v>109</v>
       </c>
       <c r="D23" s="4"/>
@@ -1679,12 +1667,15 @@
       <c r="M23" s="2"/>
       <c r="N23" s="3"/>
       <c r="O23" s="9"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="21" t="s">
         <v>110</v>
       </c>
       <c r="D24" s="4"/>
@@ -1692,7 +1683,9 @@
       <c r="F24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G24" s="2"/>
+      <c r="G24" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2" t="s">
@@ -1703,12 +1696,15 @@
       <c r="M24" s="2"/>
       <c r="N24" s="3"/>
       <c r="O24" s="9"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="21" t="s">
         <v>111</v>
       </c>
       <c r="D25" s="4"/>
@@ -1730,11 +1726,11 @@
       <c r="N25" s="3"/>
       <c r="O25" s="9"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="21" t="s">
         <v>112</v>
       </c>
       <c r="D26" s="4"/>
@@ -1742,9 +1738,7 @@
       <c r="F26" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G26" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2" t="s">
@@ -1756,11 +1750,11 @@
       <c r="N26" s="3"/>
       <c r="O26" s="9"/>
     </row>
-    <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D27" s="4"/>
@@ -1782,14 +1776,11 @@
       <c r="N27" s="3"/>
       <c r="O27" s="9"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" s="30" t="s">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B28" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="21" t="s">
         <v>114</v>
       </c>
       <c r="D28" s="4"/>
@@ -1808,16 +1799,14 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
       <c r="M28" s="2"/>
-      <c r="N28" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="N28" s="3"/>
       <c r="O28" s="9"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="21" t="s">
         <v>115</v>
       </c>
       <c r="D29" s="4"/>
@@ -1836,16 +1825,17 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="2"/>
-      <c r="N29" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="N29" s="3"/>
       <c r="O29" s="9"/>
     </row>
-    <row r="30" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="30" t="s">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="21" t="s">
         <v>116</v>
       </c>
       <c r="D30" s="4"/>
@@ -1869,149 +1859,152 @@
       </c>
       <c r="O30" s="9"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C31" s="30" t="s">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B31" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>34</v>
-      </c>
+      <c r="D31" s="4"/>
       <c r="E31" s="5"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
+      <c r="F31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="H31" s="2"/>
-      <c r="I31" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
       <c r="M31" s="2"/>
-      <c r="N31" s="3"/>
+      <c r="N31" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="O31" s="9"/>
-      <c r="T31" s="12"/>
-      <c r="U31" s="12"/>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C32" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>34</v>
-      </c>
+      <c r="D32" s="4"/>
       <c r="E32" s="5"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
+      <c r="F32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="H32" s="2"/>
-      <c r="I32" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
       <c r="M32" s="2"/>
-      <c r="N32" s="3"/>
+      <c r="N32" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="O32" s="9"/>
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B33" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C33" s="30" t="s">
+      <c r="A33" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="D33" s="4"/>
+      <c r="D33" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="E33" s="5"/>
-      <c r="F33" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="I33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J33" s="2"/>
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
       <c r="M33" s="2"/>
       <c r="N33" s="3"/>
       <c r="O33" s="9"/>
-    </row>
-    <row r="34" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T33" s="12"/>
+      <c r="U33" s="12"/>
+    </row>
+    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B34" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C34" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="D34" s="4"/>
+      <c r="D34" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="E34" s="5"/>
       <c r="F34" s="2"/>
-      <c r="G34" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="G34" s="2"/>
       <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="I34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J34" s="2"/>
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
       <c r="M34" s="2"/>
       <c r="N34" s="3"/>
       <c r="O34" s="9"/>
-      <c r="T34" s="12"/>
-      <c r="U34" s="12"/>
     </row>
     <row r="35" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="C35" s="30" t="s">
+      <c r="B35" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>34</v>
-      </c>
+      <c r="D35" s="4"/>
       <c r="E35" s="5"/>
-      <c r="F35" s="2"/>
+      <c r="F35" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
-      <c r="I35" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
       <c r="M35" s="2"/>
-      <c r="N35" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="N35" s="3"/>
       <c r="O35" s="9"/>
     </row>
     <row r="36" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="21" t="s">
         <v>122</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="5"/>
       <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
+      <c r="G36" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2" t="s">
@@ -2019,62 +2012,46 @@
       </c>
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
-      <c r="M36" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="M36" s="2"/>
       <c r="N36" s="3"/>
       <c r="O36" s="9"/>
+      <c r="T36" s="12"/>
+      <c r="U36" s="12"/>
     </row>
     <row r="37" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B37" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C37" s="30" t="s">
+      <c r="A37" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="D37" s="4"/>
+      <c r="D37" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="E37" s="5"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="I37" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J37" s="2"/>
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
-      <c r="M37" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N37" s="3"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="O37" s="9"/>
-      <c r="T37" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="U37" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="V37" s="13"/>
-      <c r="W37" s="4"/>
-      <c r="X37" s="5"/>
-      <c r="Y37" s="7"/>
-      <c r="Z37" s="7"/>
-      <c r="AA37" s="7"/>
-      <c r="AB37" s="5"/>
-      <c r="AC37" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD37" s="5"/>
-      <c r="AE37" s="5"/>
-      <c r="AF37" s="5"/>
-      <c r="AG37" s="6"/>
-      <c r="AH37" s="6"/>
     </row>
     <row r="38" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C38" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="21" t="s">
         <v>124</v>
       </c>
       <c r="D38" s="4"/>
@@ -2093,40 +2070,15 @@
       </c>
       <c r="N38" s="3"/>
       <c r="O38" s="9"/>
-      <c r="U38" t="s">
-        <v>42</v>
-      </c>
-      <c r="V38" s="13"/>
-      <c r="W38" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="X38" s="5"/>
-      <c r="Y38" s="7"/>
-      <c r="Z38" s="7"/>
-      <c r="AA38" s="7"/>
-      <c r="AB38" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC38" s="5"/>
-      <c r="AD38" s="5"/>
-      <c r="AE38" s="5"/>
-      <c r="AF38" s="5"/>
-      <c r="AG38" s="6"/>
-      <c r="AH38" s="6"/>
     </row>
     <row r="39" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A39" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C39" s="30" t="s">
+      <c r="B39" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>36</v>
-      </c>
+      <c r="D39" s="4"/>
       <c r="E39" s="5"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
@@ -2137,11 +2089,16 @@
       </c>
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
-      <c r="M39" s="2"/>
+      <c r="M39" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="N39" s="3"/>
       <c r="O39" s="9"/>
-      <c r="U39" t="s">
-        <v>60</v>
+      <c r="T39" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="U39" s="16" t="s">
+        <v>40</v>
       </c>
       <c r="V39" s="13"/>
       <c r="W39" s="4"/>
@@ -2150,44 +2107,52 @@
       <c r="Z39" s="7"/>
       <c r="AA39" s="7"/>
       <c r="AB39" s="5"/>
-      <c r="AC39" s="5"/>
+      <c r="AC39" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="AD39" s="5"/>
       <c r="AE39" s="5"/>
       <c r="AF39" s="5"/>
       <c r="AG39" s="6"/>
       <c r="AH39" s="6"/>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C40" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="D40" s="4" t="s">
-        <v>36</v>
-      </c>
+      <c r="D40" s="4"/>
       <c r="E40" s="5"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
+      <c r="J40" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
-      <c r="M40" s="2"/>
+      <c r="M40" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="N40" s="3"/>
       <c r="O40" s="9"/>
       <c r="U40" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="V40" s="13"/>
-      <c r="W40" s="4"/>
+      <c r="W40" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="X40" s="5"/>
       <c r="Y40" s="7"/>
       <c r="Z40" s="7"/>
       <c r="AA40" s="7"/>
-      <c r="AB40" s="5"/>
+      <c r="AB40" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="AC40" s="5"/>
       <c r="AD40" s="5"/>
       <c r="AE40" s="5"/>
@@ -2196,8 +2161,33 @@
       <c r="AH40" s="6"/>
     </row>
     <row r="41" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E41" s="5"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="9"/>
       <c r="U41" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="V41" s="13"/>
       <c r="W41" s="4"/>
@@ -2210,11 +2200,32 @@
       <c r="AD41" s="5"/>
       <c r="AE41" s="5"/>
       <c r="AF41" s="5"/>
-      <c r="AG41" s="5"/>
+      <c r="AG41" s="6"/>
+      <c r="AH41" s="6"/>
     </row>
     <row r="42" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B42" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E42" s="5"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="3"/>
+      <c r="O42" s="9"/>
       <c r="U42" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="V42" s="13"/>
       <c r="W42" s="4"/>
@@ -2227,60 +2238,72 @@
       <c r="AD42" s="5"/>
       <c r="AE42" s="5"/>
       <c r="AF42" s="5"/>
-      <c r="AG42" s="5"/>
+      <c r="AG42" s="6"/>
+      <c r="AH42" s="6"/>
     </row>
     <row r="43" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="T43" s="12"/>
-      <c r="U43" s="12"/>
-    </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="T47" s="12"/>
-      <c r="U47" s="12"/>
-    </row>
-    <row r="52" spans="20:21" x14ac:dyDescent="0.25">
-      <c r="T52" s="12"/>
-      <c r="U52" s="12"/>
-    </row>
-    <row r="57" spans="20:21" x14ac:dyDescent="0.25">
-      <c r="T57" s="12"/>
-      <c r="U57" s="12"/>
-    </row>
-    <row r="74" spans="16:24" x14ac:dyDescent="0.25">
-      <c r="P74" s="22"/>
-      <c r="Q74" s="22"/>
-      <c r="R74" s="22"/>
-      <c r="S74" s="22"/>
-      <c r="T74" s="22"/>
-      <c r="U74" s="22"/>
-      <c r="V74" s="22"/>
-      <c r="W74" s="22"/>
-      <c r="X74" s="21"/>
-    </row>
-    <row r="75" spans="16:24" x14ac:dyDescent="0.25">
-      <c r="P75" s="21"/>
-      <c r="Q75" s="21"/>
-      <c r="R75" s="21"/>
-      <c r="S75" s="21"/>
-      <c r="T75" s="21"/>
-      <c r="U75" s="21"/>
-      <c r="V75" s="21"/>
-      <c r="W75" s="21"/>
-      <c r="X75" s="21"/>
-    </row>
-    <row r="76" spans="16:24" x14ac:dyDescent="0.25">
-      <c r="P76" s="21"/>
-      <c r="Q76" s="21"/>
-      <c r="R76" s="21"/>
-      <c r="S76" s="21"/>
-      <c r="T76" s="21"/>
-      <c r="U76" s="21"/>
-      <c r="V76" s="21"/>
-      <c r="W76" s="21"/>
-      <c r="X76" s="21"/>
+      <c r="U43" t="s">
+        <v>62</v>
+      </c>
+      <c r="V43" s="13"/>
+      <c r="W43" s="4"/>
+      <c r="X43" s="5"/>
+      <c r="Y43" s="7"/>
+      <c r="Z43" s="7"/>
+      <c r="AA43" s="7"/>
+      <c r="AB43" s="5"/>
+      <c r="AC43" s="5"/>
+      <c r="AD43" s="5"/>
+      <c r="AE43" s="5"/>
+      <c r="AF43" s="5"/>
+      <c r="AG43" s="5"/>
+    </row>
+    <row r="44" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="U44" t="s">
+        <v>63</v>
+      </c>
+      <c r="V44" s="13"/>
+      <c r="W44" s="4"/>
+      <c r="X44" s="5"/>
+      <c r="Y44" s="7"/>
+      <c r="Z44" s="7"/>
+      <c r="AA44" s="7"/>
+      <c r="AB44" s="5"/>
+      <c r="AC44" s="5"/>
+      <c r="AD44" s="5"/>
+      <c r="AE44" s="5"/>
+      <c r="AF44" s="5"/>
+      <c r="AG44" s="5"/>
+    </row>
+    <row r="45" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="T45" s="12"/>
+      <c r="U45" s="12"/>
+    </row>
+    <row r="49" spans="20:21" x14ac:dyDescent="0.25">
+      <c r="T49" s="12"/>
+      <c r="U49" s="12"/>
+    </row>
+    <row r="54" spans="20:21" x14ac:dyDescent="0.25">
+      <c r="T54" s="12"/>
+      <c r="U54" s="12"/>
+    </row>
+    <row r="59" spans="20:21" x14ac:dyDescent="0.25">
+      <c r="T59" s="12"/>
+      <c r="U59" s="12"/>
+    </row>
+    <row r="76" spans="16:23" x14ac:dyDescent="0.25">
+      <c r="P76" s="12"/>
+      <c r="Q76" s="12"/>
+      <c r="R76" s="12"/>
+      <c r="S76" s="12"/>
+      <c r="T76" s="12"/>
+      <c r="U76" s="12"/>
+      <c r="V76" s="12"/>
+      <c r="W76" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2304,10 +2327,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="19"/>
+      <c r="B2" s="27"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2354,10 +2377,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="19"/>
+      <c r="B13" s="27"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">

</xml_diff>

<commit_message>
finished lookup table, still needs testing
not sure on the actual operation
</commit_message>
<xml_diff>
--- a/8Bit Computer ver2.0/excel/commands.xlsx
+++ b/8Bit Computer ver2.0/excel/commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\GitHub\Private\Computer_HTL\8Bit Computer ver2.0\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD0172F-215F-4AA3-822B-228DF47E29EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA26BE71-B44F-4674-9D55-8F4877EB130B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3256ACAE-F419-450F-8F49-2183F1DCCADE}"/>
+    <workbookView xWindow="38295" yWindow="10905" windowWidth="16410" windowHeight="14145" xr2:uid="{3256ACAE-F419-450F-8F49-2183F1DCCADE}"/>
   </bookViews>
   <sheets>
     <sheet name="Commands" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="130">
   <si>
     <t>NOP</t>
   </si>
@@ -238,12 +238,6 @@
     <t>&gt; best solution</t>
   </si>
   <si>
-    <t>A/B REGISTER</t>
-  </si>
-  <si>
-    <t>C REGISTER</t>
-  </si>
-  <si>
     <t>STORE C</t>
   </si>
   <si>
@@ -419,6 +413,9 @@
   </si>
   <si>
     <t>STORE to register 1</t>
+  </si>
+  <si>
+    <t>A/B/C REGISTER</t>
   </si>
 </sst>
 </file>
@@ -601,7 +598,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -668,6 +665,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1004,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02BDFC33-BE10-4835-94A0-E5C8BC037442}">
   <dimension ref="A1:AH76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,7 +1029,7 @@
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>30</v>
@@ -1078,7 +1076,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="5"/>
@@ -1098,7 +1096,7 @@
         <v>66</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="5" t="s">
@@ -1127,7 +1125,7 @@
         <v>65</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="5" t="s">
@@ -1155,10 +1153,10 @@
         <v>39</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="5"/>
@@ -1180,10 +1178,10 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="5"/>
@@ -1208,7 +1206,7 @@
         <v>42</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="5" t="s">
@@ -1232,7 +1230,7 @@
         <v>40</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="5" t="s">
@@ -1253,10 +1251,10 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>35</v>
@@ -1280,10 +1278,10 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>35</v>
@@ -1304,10 +1302,10 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="5"/>
@@ -1324,10 +1322,10 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="5"/>
@@ -1347,7 +1345,7 @@
         <v>41</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="5" t="s">
@@ -1372,7 +1370,7 @@
       </c>
       <c r="B14" s="23"/>
       <c r="C14" s="19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D14" s="19" t="s">
         <v>30</v>
@@ -1419,7 +1417,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="5"/>
@@ -1447,7 +1445,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="5"/>
@@ -1477,7 +1475,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="5"/>
@@ -1508,7 +1506,7 @@
         <v>6</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="5"/>
@@ -1519,7 +1517,7 @@
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
@@ -1534,7 +1532,7 @@
         <v>7</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="5"/>
@@ -1545,7 +1543,7 @@
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
@@ -1560,25 +1558,25 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>34</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="D20" s="4"/>
       <c r="E20" s="5"/>
-      <c r="F20" s="2"/>
+      <c r="F20" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="2"/>
@@ -1588,20 +1586,22 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="5"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="F21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2" t="s">
         <v>10</v>
@@ -1616,21 +1616,20 @@
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>22</v>
+      <c r="B22" s="10" t="s">
+        <v>24</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="5"/>
       <c r="F22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2" t="s">
@@ -1644,10 +1643,10 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="5"/>
@@ -1673,19 +1672,17 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="5"/>
       <c r="F24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2" t="s">
@@ -1702,10 +1699,10 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="5"/>
@@ -1728,17 +1725,19 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="5"/>
       <c r="F26" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G26" s="2"/>
+      <c r="G26" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2" t="s">
@@ -1750,12 +1749,12 @@
       <c r="N26" s="3"/>
       <c r="O26" s="9"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="5"/>
@@ -1777,11 +1776,14 @@
       <c r="O27" s="9"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B28" s="10" t="s">
-        <v>28</v>
+      <c r="A28" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="5"/>
@@ -1799,15 +1801,17 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
       <c r="M28" s="2"/>
-      <c r="N28" s="3"/>
+      <c r="N28" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="O28" s="9"/>
     </row>
-    <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="5"/>
@@ -1825,18 +1829,17 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="2"/>
-      <c r="N29" s="3"/>
+      <c r="N29" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="O29" s="9"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>51</v>
+    <row r="30" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="5"/>
@@ -1860,48 +1863,45 @@
       <c r="O30" s="9"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B31" s="10" t="s">
-        <v>50</v>
+      <c r="A31" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="D31" s="4"/>
+        <v>113</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="E31" s="5"/>
-      <c r="F31" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
       <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="I31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J31" s="2"/>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
       <c r="M31" s="2"/>
-      <c r="N31" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="N31" s="3"/>
       <c r="O31" s="9"/>
     </row>
-    <row r="32" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B32" s="10" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="5"/>
       <c r="F32" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G32" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2" t="s">
@@ -1910,20 +1910,15 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
       <c r="M32" s="2"/>
-      <c r="N32" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="N32" s="3"/>
       <c r="O32" s="9"/>
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>73</v>
+      <c r="B33" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>34</v>
@@ -1946,17 +1941,17 @@
     </row>
     <row r="34" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B34" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="5"/>
-      <c r="F34" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2" t="s">
@@ -1969,11 +1964,12 @@
       <c r="O34" s="9"/>
     </row>
     <row r="35" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B35" s="10" t="s">
-        <v>74</v>
+      <c r="A35" s="28"/>
+      <c r="B35" s="18" t="s">
+        <v>70</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>34</v>
@@ -1994,18 +1990,18 @@
     </row>
     <row r="36" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="10" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="5"/>
       <c r="F36" s="2"/>
-      <c r="G36" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2" t="s">
         <v>10</v>
@@ -2023,10 +2019,10 @@
         <v>20</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>34</v>
@@ -2049,10 +2045,10 @@
     </row>
     <row r="38" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="5"/>
@@ -2073,10 +2069,10 @@
     </row>
     <row r="39" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B39" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="5"/>
@@ -2121,7 +2117,7 @@
         <v>8</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="5"/>
@@ -2165,10 +2161,10 @@
         <v>21</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>36</v>
@@ -2205,10 +2201,10 @@
     </row>
     <row r="42" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B42" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
added data to address bus interface
</commit_message>
<xml_diff>
--- a/8Bit Computer ver2.0/excel/commands.xlsx
+++ b/8Bit Computer ver2.0/excel/commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\GitHub\Private\Computer_HTL\8Bit Computer ver2.0\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91D5D79-DFDA-40FB-A57F-FCF7D4F8C8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94C5F91-CF1A-4C70-9289-A605A32CD25B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12930" yWindow="5865" windowWidth="16410" windowHeight="16005" xr2:uid="{3256ACAE-F419-450F-8F49-2183F1DCCADE}"/>
+    <workbookView xWindow="3570" yWindow="1305" windowWidth="17820" windowHeight="18345" xr2:uid="{3256ACAE-F419-450F-8F49-2183F1DCCADE}"/>
   </bookViews>
   <sheets>
     <sheet name="Commands" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="118">
   <si>
     <t>NOP</t>
   </si>
@@ -73,9 +73,6 @@
     <t>1 tick delay</t>
   </si>
   <si>
-    <t>multiplexer</t>
-  </si>
-  <si>
     <t>&gt; needs 1 d-latch and bus interface per operation</t>
   </si>
   <si>
@@ -151,9 +148,6 @@
     <t>LOAD</t>
   </si>
   <si>
-    <t>LOAD to address bus</t>
-  </si>
-  <si>
     <t>STORE</t>
   </si>
   <si>
@@ -205,21 +199,9 @@
     <t>TIMER</t>
   </si>
   <si>
-    <t>CLEAR</t>
-  </si>
-  <si>
-    <t>STOP</t>
-  </si>
-  <si>
     <t>comparison true</t>
   </si>
   <si>
-    <t>STORE to comparison reg</t>
-  </si>
-  <si>
-    <t>CLEAR comparison reg</t>
-  </si>
-  <si>
     <t>To PC</t>
   </si>
   <si>
@@ -277,12 +259,6 @@
     <t>HEX</t>
   </si>
   <si>
-    <t>STORE to data (address from register 1 + 2)</t>
-  </si>
-  <si>
-    <t>LOAD from data (address from register 1 + 2)</t>
-  </si>
-  <si>
     <t>0x00</t>
   </si>
   <si>
@@ -391,31 +367,19 @@
     <t>0x23</t>
   </si>
   <si>
-    <t>0x24</t>
-  </si>
-  <si>
-    <t>0x25</t>
-  </si>
-  <si>
-    <t>LOAD to register 1 (for output to addr bus)</t>
-  </si>
-  <si>
-    <t>LOAD to register 2 (for output to addr bus)</t>
-  </si>
-  <si>
-    <t>0x26</t>
-  </si>
-  <si>
-    <t>0x27</t>
-  </si>
-  <si>
-    <t>STORE to register 2</t>
-  </si>
-  <si>
-    <t>STORE to register 1</t>
-  </si>
-  <si>
     <t>A/B/C REGISTER</t>
+  </si>
+  <si>
+    <t>val_16</t>
+  </si>
+  <si>
+    <t>STORE to interface register 1</t>
+  </si>
+  <si>
+    <t>STORE to interface register 2</t>
+  </si>
+  <si>
+    <t>LOAD from interface registers</t>
   </si>
 </sst>
 </file>
@@ -444,7 +408,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -475,14 +439,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -600,11 +558,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -638,10 +616,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -671,8 +647,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1007,10 +990,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02BDFC33-BE10-4835-94A0-E5C8BC037442}">
-  <dimension ref="A1:AH76"/>
+  <dimension ref="A1:AH72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,48 +1014,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" s="19" t="s">
+      <c r="A1" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="19" t="s">
+      <c r="H1" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="K1" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="L1" s="19" t="s">
+      <c r="N1" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="M1" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="N1" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="O1" s="20" t="s">
-        <v>64</v>
+      <c r="O1" s="18" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1082,8 +1065,8 @@
       <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="21" t="s">
-        <v>85</v>
+      <c r="C2" s="19" t="s">
+        <v>77</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="5"/>
@@ -1100,14 +1083,14 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>86</v>
+        <v>60</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>78</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -1127,16 +1110,16 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>87</v>
+        <v>59</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>79</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -1156,288 +1139,313 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
+      <c r="B5" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="1"/>
       <c r="Q5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="5"/>
+      <c r="B6" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
-      <c r="I6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
+      <c r="I6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="1"/>
       <c r="Q6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>90</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="26"/>
+      <c r="B7" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>82</v>
       </c>
       <c r="D7" s="4"/>
-      <c r="E7" s="5" t="s">
-        <v>35</v>
+      <c r="E7" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="1"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="18" t="s">
+      <c r="A8" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="21" t="s">
-        <v>91</v>
+      <c r="C8" s="19" t="s">
+        <v>83</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="I8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="5"/>
+    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="J9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="5"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
-      <c r="Q9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
+    </row>
+    <row r="10" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="C10" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="K10" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="L10" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="M10" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="N10" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="O10" s="18" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>94</v>
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>85</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="5"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
+      <c r="F11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O11" s="9"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>95</v>
+      <c r="B12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>86</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
+      <c r="F12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
+      <c r="M12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O12" s="9"/>
     </row>
     <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O13" s="9"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M13" s="5"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-    </row>
-    <row r="14" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="23"/>
+      <c r="B14" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="C14" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="I14" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="J14" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="K14" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="L14" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="M14" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="N14" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="O14" s="20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>97</v>
+        <v>88</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O14" s="9"/>
+    </row>
+    <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>89</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
@@ -1446,22 +1454,26 @@
         <v>10</v>
       </c>
       <c r="O15" s="9"/>
+      <c r="Q15" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>98</v>
+      <c r="A16" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>90</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="5"/>
       <c r="F16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2" t="s">
@@ -1469,20 +1481,19 @@
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
-      <c r="M16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N16" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="M16" s="2"/>
+      <c r="N16" s="3"/>
       <c r="O16" s="9"/>
-    </row>
-    <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>99</v>
+        <v>22</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>91</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="5"/>
@@ -1500,78 +1511,73 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
       <c r="M17" s="2"/>
-      <c r="N17" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="N17" s="3"/>
       <c r="O17" s="9"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>100</v>
+      <c r="Q17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B18" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>92</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="F18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="2"/>
-      <c r="N18" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="N18" s="3"/>
       <c r="O18" s="9"/>
     </row>
-    <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="21" t="s">
-        <v>101</v>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B19" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>93</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="F19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="2"/>
-      <c r="N19" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="N19" s="3"/>
       <c r="O19" s="9"/>
       <c r="Q19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>102</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B20" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>94</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="5"/>
@@ -1590,15 +1596,15 @@
       <c r="N20" s="3"/>
       <c r="O20" s="9"/>
       <c r="Q20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>103</v>
+        <v>26</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>95</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="5"/>
@@ -1618,16 +1624,13 @@
       <c r="M21" s="2"/>
       <c r="N21" s="3"/>
       <c r="O21" s="9"/>
-      <c r="Q21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>104</v>
+        <v>27</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>96</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="5"/>
@@ -1648,12 +1651,12 @@
       <c r="N22" s="3"/>
       <c r="O22" s="9"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="21" t="s">
-        <v>105</v>
+        <v>28</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>97</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="5"/>
@@ -1673,23 +1676,25 @@
       <c r="M23" s="2"/>
       <c r="N23" s="3"/>
       <c r="O23" s="9"/>
-      <c r="Q23" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B24" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>106</v>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>98</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="5"/>
       <c r="F24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G24" s="2"/>
+      <c r="G24" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2" t="s">
@@ -1698,18 +1703,17 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="2"/>
-      <c r="N24" s="3"/>
+      <c r="N24" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="O24" s="9"/>
-      <c r="Q24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>107</v>
+        <v>48</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>99</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="5"/>
@@ -1727,15 +1731,17 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="2"/>
-      <c r="N25" s="3"/>
+      <c r="N25" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="O25" s="9"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>108</v>
+        <v>50</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>100</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="5"/>
@@ -1753,53 +1759,51 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
       <c r="M26" s="2"/>
-      <c r="N26" s="3"/>
+      <c r="N26" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="O26" s="9"/>
     </row>
-    <row r="27" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="D27" s="4"/>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="E27" s="5"/>
-      <c r="F27" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
       <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="I27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J27" s="2"/>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="M27" s="2"/>
       <c r="N27" s="3"/>
       <c r="O27" s="9"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" s="21" t="s">
-        <v>110</v>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B28" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>102</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="5"/>
       <c r="F28" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2" t="s">
@@ -1808,51 +1812,45 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
       <c r="M28" s="2"/>
-      <c r="N28" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="N28" s="3"/>
       <c r="O28" s="9"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="D29" s="4"/>
+        <v>66</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="E29" s="5"/>
-      <c r="F29" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
       <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="I29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J29" s="2"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="2"/>
-      <c r="N29" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="N29" s="3"/>
       <c r="O29" s="9"/>
-    </row>
-    <row r="30" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T29" s="12"/>
+      <c r="U29" s="12"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="21" t="s">
-        <v>112</v>
+        <v>73</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>104</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="5"/>
-      <c r="F30" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="F30" s="2"/>
       <c r="G30" s="2" t="s">
         <v>10</v>
       </c>
@@ -1864,23 +1862,18 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
       <c r="M30" s="2"/>
-      <c r="N30" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="N30" s="3"/>
       <c r="O30" s="9"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="C31" s="21" t="s">
-        <v>113</v>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B31" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>105</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="2"/>
@@ -1896,20 +1889,20 @@
       <c r="N31" s="3"/>
       <c r="O31" s="9"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C32" s="21" t="s">
-        <v>114</v>
+        <v>70</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>106</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="5"/>
-      <c r="F32" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="F32" s="2"/>
       <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
+      <c r="H32" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2" t="s">
         <v>10</v>
@@ -1919,16 +1912,21 @@
       <c r="M32" s="2"/>
       <c r="N32" s="3"/>
       <c r="O32" s="9"/>
+      <c r="T32" s="12"/>
+      <c r="U32" s="12"/>
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B33" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>115</v>
+      <c r="A33" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>107</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="2"/>
@@ -1941,24 +1939,22 @@
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
       <c r="M33" s="2"/>
-      <c r="N33" s="3"/>
+      <c r="N33" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="O33" s="9"/>
-      <c r="T33" s="12"/>
-      <c r="U33" s="12"/>
     </row>
     <row r="34" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B34" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C34" s="21" t="s">
-        <v>116</v>
+        <v>68</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>108</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="5"/>
       <c r="F34" s="2"/>
-      <c r="G34" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2" t="s">
@@ -1966,346 +1962,263 @@
       </c>
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
-      <c r="M34" s="2"/>
+      <c r="M34" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="N34" s="3"/>
       <c r="O34" s="9"/>
+      <c r="T34" s="28"/>
+      <c r="U34" s="28"/>
+      <c r="V34" s="28"/>
+      <c r="W34" s="28"/>
+      <c r="X34" s="28"/>
+      <c r="Y34" s="28"/>
+      <c r="Z34" s="28"/>
+      <c r="AA34" s="28"/>
+      <c r="AB34" s="28"/>
+      <c r="AC34" s="28"/>
+      <c r="AD34" s="28"/>
     </row>
     <row r="35" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B35" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C35" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>34</v>
-      </c>
+      <c r="B35" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" s="4"/>
       <c r="E35" s="5"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
-      <c r="I35" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
-      <c r="M35" s="2"/>
+      <c r="M35" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="N35" s="3"/>
       <c r="O35" s="9"/>
+      <c r="T35" s="28"/>
+      <c r="U35" s="28"/>
+      <c r="V35" s="28"/>
+      <c r="W35" s="29"/>
+      <c r="X35" s="29"/>
+      <c r="Y35" s="30"/>
+      <c r="Z35" s="30"/>
+      <c r="AA35" s="30"/>
+      <c r="AB35" s="29"/>
+      <c r="AC35" s="29"/>
+      <c r="AD35" s="29"/>
+      <c r="AE35" s="29"/>
+      <c r="AF35" s="29"/>
+      <c r="AG35" s="29"/>
+      <c r="AH35" s="29"/>
     </row>
     <row r="36" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C36" s="21" t="s">
-        <v>118</v>
+        <v>8</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>110</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="5"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2" t="s">
         <v>10</v>
       </c>
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
-      <c r="M36" s="2"/>
+      <c r="M36" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="N36" s="3"/>
       <c r="O36" s="9"/>
-      <c r="T36" s="12"/>
-      <c r="U36" s="12"/>
+      <c r="T36" s="28"/>
+      <c r="U36" s="28"/>
+      <c r="V36" s="28"/>
+      <c r="W36" s="29"/>
+      <c r="X36" s="29"/>
+      <c r="Y36" s="30"/>
+      <c r="Z36" s="30"/>
+      <c r="AA36" s="30"/>
+      <c r="AB36" s="29"/>
+      <c r="AC36" s="29"/>
+      <c r="AD36" s="29"/>
+      <c r="AE36" s="29"/>
+      <c r="AF36" s="29"/>
+      <c r="AG36" s="29"/>
+      <c r="AH36" s="29"/>
     </row>
     <row r="37" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B37" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C37" s="21" t="s">
-        <v>119</v>
+      <c r="B37" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>111</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
-      <c r="I37" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
       <c r="M37" s="2"/>
-      <c r="N37" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="N37" s="3"/>
       <c r="O37" s="9"/>
-    </row>
-    <row r="38" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T37" s="28"/>
+      <c r="U37" s="28"/>
+      <c r="V37" s="28"/>
+      <c r="W37" s="29"/>
+      <c r="X37" s="29"/>
+      <c r="Y37" s="30"/>
+      <c r="Z37" s="30"/>
+      <c r="AA37" s="30"/>
+      <c r="AB37" s="29"/>
+      <c r="AC37" s="29"/>
+      <c r="AD37" s="29"/>
+      <c r="AE37" s="29"/>
+      <c r="AF37" s="29"/>
+      <c r="AG37" s="29"/>
+      <c r="AH37" s="29"/>
+    </row>
+    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B38" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C38" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="D38" s="4"/>
+        <v>75</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="E38" s="5"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
-      <c r="J38" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="J38" s="2"/>
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
-      <c r="M38" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="M38" s="2"/>
       <c r="N38" s="3"/>
       <c r="O38" s="9"/>
+      <c r="T38" s="28"/>
+      <c r="U38" s="28"/>
+      <c r="V38" s="28"/>
+      <c r="W38" s="29"/>
+      <c r="X38" s="29"/>
+      <c r="Y38" s="30"/>
+      <c r="Z38" s="30"/>
+      <c r="AA38" s="30"/>
+      <c r="AB38" s="29"/>
+      <c r="AC38" s="29"/>
+      <c r="AD38" s="29"/>
+      <c r="AE38" s="29"/>
+      <c r="AF38" s="29"/>
+      <c r="AG38" s="29"/>
+      <c r="AH38" s="29"/>
     </row>
     <row r="39" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B39" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C39" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K39" s="5"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N39" s="3"/>
-      <c r="O39" s="9"/>
-      <c r="T39" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="U39" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="V39" s="13"/>
-      <c r="W39" s="4"/>
-      <c r="X39" s="5"/>
-      <c r="Y39" s="7"/>
-      <c r="Z39" s="7"/>
-      <c r="AA39" s="7"/>
-      <c r="AB39" s="5"/>
-      <c r="AC39" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD39" s="5"/>
-      <c r="AE39" s="5"/>
-      <c r="AF39" s="5"/>
-      <c r="AG39" s="6"/>
-      <c r="AH39" s="6"/>
-    </row>
-    <row r="40" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="D40" s="4"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K40" s="5"/>
-      <c r="L40" s="5"/>
-      <c r="M40" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N40" s="3"/>
-      <c r="O40" s="9"/>
-      <c r="U40" t="s">
-        <v>42</v>
-      </c>
-      <c r="V40" s="13"/>
-      <c r="W40" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="X40" s="5"/>
-      <c r="Y40" s="7"/>
-      <c r="Z40" s="7"/>
-      <c r="AA40" s="7"/>
-      <c r="AB40" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC40" s="5"/>
-      <c r="AD40" s="5"/>
-      <c r="AE40" s="5"/>
-      <c r="AF40" s="5"/>
-      <c r="AG40" s="6"/>
-      <c r="AH40" s="6"/>
+      <c r="T39" s="28"/>
+      <c r="U39" s="28"/>
+      <c r="V39" s="28"/>
+      <c r="W39" s="29"/>
+      <c r="X39" s="29"/>
+      <c r="Y39" s="30"/>
+      <c r="Z39" s="30"/>
+      <c r="AA39" s="30"/>
+      <c r="AB39" s="29"/>
+      <c r="AC39" s="29"/>
+      <c r="AD39" s="29"/>
+      <c r="AE39" s="29"/>
+      <c r="AF39" s="29"/>
+      <c r="AG39" s="29"/>
+    </row>
+    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="T40" s="28"/>
+      <c r="U40" s="28"/>
+      <c r="V40" s="28"/>
+      <c r="W40" s="29"/>
+      <c r="X40" s="29"/>
+      <c r="Y40" s="30"/>
+      <c r="Z40" s="30"/>
+      <c r="AA40" s="30"/>
+      <c r="AB40" s="29"/>
+      <c r="AC40" s="29"/>
+      <c r="AD40" s="29"/>
+      <c r="AE40" s="29"/>
+      <c r="AF40" s="29"/>
+      <c r="AG40" s="29"/>
     </row>
     <row r="41" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C41" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E41" s="5"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K41" s="5"/>
-      <c r="L41" s="5"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="3"/>
-      <c r="O41" s="9"/>
-      <c r="U41" t="s">
-        <v>60</v>
-      </c>
-      <c r="V41" s="13"/>
-      <c r="W41" s="4"/>
-      <c r="X41" s="5"/>
-      <c r="Y41" s="7"/>
-      <c r="Z41" s="7"/>
-      <c r="AA41" s="7"/>
-      <c r="AB41" s="5"/>
-      <c r="AC41" s="5"/>
-      <c r="AD41" s="5"/>
-      <c r="AE41" s="5"/>
-      <c r="AF41" s="5"/>
-      <c r="AG41" s="6"/>
-      <c r="AH41" s="6"/>
+      <c r="T41" s="29"/>
+      <c r="U41" s="29"/>
+      <c r="V41" s="28"/>
+      <c r="W41" s="28"/>
+      <c r="X41" s="28"/>
+      <c r="Y41" s="28"/>
+      <c r="Z41" s="28"/>
+      <c r="AA41" s="28"/>
+      <c r="AB41" s="28"/>
+      <c r="AC41" s="28"/>
+      <c r="AD41" s="28"/>
     </row>
     <row r="42" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B42" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C42" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E42" s="5"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="5"/>
-      <c r="L42" s="5"/>
-      <c r="M42" s="2"/>
-      <c r="N42" s="3"/>
-      <c r="O42" s="9"/>
-      <c r="U42" t="s">
-        <v>59</v>
-      </c>
-      <c r="V42" s="13"/>
-      <c r="W42" s="4"/>
-      <c r="X42" s="5"/>
-      <c r="Y42" s="7"/>
-      <c r="Z42" s="7"/>
-      <c r="AA42" s="7"/>
-      <c r="AB42" s="5"/>
-      <c r="AC42" s="5"/>
-      <c r="AD42" s="5"/>
-      <c r="AE42" s="5"/>
-      <c r="AF42" s="5"/>
-      <c r="AG42" s="6"/>
-      <c r="AH42" s="6"/>
-    </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="U43" t="s">
-        <v>62</v>
-      </c>
-      <c r="V43" s="13"/>
-      <c r="W43" s="4"/>
-      <c r="X43" s="5"/>
-      <c r="Y43" s="7"/>
-      <c r="Z43" s="7"/>
-      <c r="AA43" s="7"/>
-      <c r="AB43" s="5"/>
-      <c r="AC43" s="5"/>
-      <c r="AD43" s="5"/>
-      <c r="AE43" s="5"/>
-      <c r="AF43" s="5"/>
-      <c r="AG43" s="5"/>
-    </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="U44" t="s">
-        <v>63</v>
-      </c>
-      <c r="V44" s="13"/>
-      <c r="W44" s="4"/>
-      <c r="X44" s="5"/>
-      <c r="Y44" s="7"/>
-      <c r="Z44" s="7"/>
-      <c r="AA44" s="7"/>
-      <c r="AB44" s="5"/>
-      <c r="AC44" s="5"/>
-      <c r="AD44" s="5"/>
-      <c r="AE44" s="5"/>
-      <c r="AF44" s="5"/>
-      <c r="AG44" s="5"/>
+      <c r="T42" s="28"/>
+      <c r="U42" s="28"/>
+      <c r="V42" s="28"/>
+      <c r="W42" s="28"/>
+      <c r="X42" s="28"/>
+      <c r="Y42" s="28"/>
+      <c r="Z42" s="28"/>
+      <c r="AA42" s="28"/>
+      <c r="AB42" s="28"/>
+      <c r="AC42" s="28"/>
+      <c r="AD42" s="28"/>
     </row>
     <row r="45" spans="1:34" x14ac:dyDescent="0.25">
       <c r="T45" s="12"/>
       <c r="U45" s="12"/>
     </row>
-    <row r="49" spans="20:21" x14ac:dyDescent="0.25">
-      <c r="T49" s="12"/>
-      <c r="U49" s="12"/>
-    </row>
-    <row r="54" spans="20:21" x14ac:dyDescent="0.25">
-      <c r="T54" s="12"/>
-      <c r="U54" s="12"/>
-    </row>
-    <row r="59" spans="20:21" x14ac:dyDescent="0.25">
-      <c r="T59" s="12"/>
-      <c r="U59" s="12"/>
-    </row>
-    <row r="76" spans="16:23" x14ac:dyDescent="0.25">
-      <c r="P76" s="12"/>
-      <c r="Q76" s="12"/>
-      <c r="R76" s="12"/>
-      <c r="S76" s="12"/>
-      <c r="T76" s="12"/>
-      <c r="U76" s="12"/>
-      <c r="V76" s="12"/>
-      <c r="W76" s="12"/>
+    <row r="50" spans="20:21" x14ac:dyDescent="0.25">
+      <c r="T50" s="12"/>
+      <c r="U50" s="12"/>
+    </row>
+    <row r="55" spans="20:21" x14ac:dyDescent="0.25">
+      <c r="T55" s="12"/>
+      <c r="U55" s="12"/>
+    </row>
+    <row r="72" spans="16:23" x14ac:dyDescent="0.25">
+      <c r="P72" s="12"/>
+      <c r="Q72" s="12"/>
+      <c r="R72" s="12"/>
+      <c r="S72" s="12"/>
+      <c r="T72" s="12"/>
+      <c r="U72" s="12"/>
+      <c r="V72" s="12"/>
+      <c r="W72" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A10:B10"/>
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2329,72 +2242,72 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="27"/>
+      <c r="A2" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="25"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="27"/>
+      <c r="A13" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="25"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added register in front of the shift reg
would have caused a bus collision
 otherwise
</commit_message>
<xml_diff>
--- a/8Bit Computer ver2.0/excel/commands.xlsx
+++ b/8Bit Computer ver2.0/excel/commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\GitHub\Private\Computer_HTL\8Bit Computer ver2.0\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821D9A65-C615-4A14-9C79-68DBDC9438B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054670C4-AEDA-4F32-BDCE-D33F7A630A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3256ACAE-F419-450F-8F49-2183F1DCCADE}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="145">
   <si>
     <t>NOP</t>
   </si>
@@ -133,9 +133,6 @@
     <t>addr</t>
   </si>
   <si>
-    <t>distance</t>
-  </si>
-  <si>
     <t>ALU</t>
   </si>
   <si>
@@ -370,9 +367,6 @@
     <t>A/B/C REGISTER</t>
   </si>
   <si>
-    <t>val_16</t>
-  </si>
-  <si>
     <t>STORE to interface register 1</t>
   </si>
   <si>
@@ -416,6 +410,57 @@
   </si>
   <si>
     <t>BUS TRANSFER</t>
+  </si>
+  <si>
+    <t>0x27</t>
+  </si>
+  <si>
+    <t>LOAD UNREAD</t>
+  </si>
+  <si>
+    <t>unread_1b</t>
+  </si>
+  <si>
+    <t>carry_1b</t>
+  </si>
+  <si>
+    <t>val_16b</t>
+  </si>
+  <si>
+    <t>ovflw_1b</t>
+  </si>
+  <si>
+    <t>flags_2b</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>out</t>
+  </si>
+  <si>
+    <t>out_1b</t>
+  </si>
+  <si>
+    <t>no value on bus</t>
+  </si>
+  <si>
+    <t>value in current cycle (usually as an input to the current command)</t>
+  </si>
+  <si>
+    <t>value in next cycle (usually the output from the current command)</t>
+  </si>
+  <si>
+    <t>0x28</t>
+  </si>
+  <si>
+    <t>0x29</t>
+  </si>
+  <si>
+    <t>STORE DISTANCE</t>
+  </si>
+  <si>
+    <t>LOAD DISTANCE</t>
   </si>
 </sst>
 </file>
@@ -444,7 +489,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -475,8 +520,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -614,11 +677,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -628,9 +736,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -667,6 +772,46 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -685,19 +830,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1037,7 +1176,7 @@
   <dimension ref="A1:AH72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B10"/>
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1055,149 +1194,159 @@
     <col min="12" max="12" width="9" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
     <col min="14" max="14" width="9.7109375" customWidth="1"/>
+    <col min="17" max="17" width="67.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="D1" s="17" t="s">
+      <c r="A1" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="K1" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="L1" s="17" t="s">
+      <c r="M1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="N1" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="N1" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="O1" s="18" t="s">
-        <v>58</v>
+      <c r="O1" s="17" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="Q2" s="41" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="19" t="s">
+      <c r="D3" s="28"/>
+      <c r="E3" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="42" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5" t="s">
+      <c r="D4" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="E4" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="19" t="s">
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q4" s="43" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
       <c r="I5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1207,23 +1356,22 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="1"/>
-      <c r="Q5" t="s">
-        <v>14</v>
-      </c>
+      <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="B6" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
       <c r="I6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1233,25 +1381,23 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="1"/>
-      <c r="Q6" t="s">
-        <v>15</v>
-      </c>
+      <c r="Q6" s="1"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
-      <c r="B7" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="28"/>
+      <c r="E7" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
       <c r="I7" s="1"/>
       <c r="J7" s="2"/>
       <c r="K7" s="1"/>
@@ -1261,115 +1407,125 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="1"/>
+      <c r="Q7" s="1"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="Q8" s="1"/>
+    </row>
+    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="19" t="s">
+      <c r="C9" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5" t="s">
+      <c r="D9" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-    </row>
-    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="D10" s="17" t="s">
+      <c r="A10" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="36"/>
+      <c r="C10" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="I10" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="K10" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="L10" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="J10" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="K10" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="L10" s="17" t="s">
+      <c r="M10" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="M10" s="17" t="s">
+      <c r="N10" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="N10" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="O10" s="18" t="s">
-        <v>58</v>
-      </c>
+      <c r="O10" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q10" s="1"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="5"/>
+      <c r="C11" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="E11" s="29"/>
       <c r="F11" s="2" t="s">
         <v>10</v>
       </c>
@@ -1381,23 +1537,26 @@
       <c r="J11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
       <c r="M11" s="2"/>
       <c r="N11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="O11" s="9"/>
+      <c r="O11" s="8"/>
+      <c r="Q11" s="1"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="5"/>
+      <c r="C12" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="E12" s="29"/>
       <c r="F12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1409,25 +1568,28 @@
       <c r="J12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
       <c r="M12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="N12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="O12" s="9"/>
+      <c r="O12" s="8"/>
+      <c r="Q12" s="1"/>
     </row>
     <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="5"/>
+      <c r="C13" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="E13" s="29"/>
       <c r="F13" s="2" t="s">
         <v>10</v>
       </c>
@@ -1439,26 +1601,31 @@
       <c r="J13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
       <c r="M13" s="2"/>
       <c r="N13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="O13" s="9"/>
+      <c r="O13" s="8"/>
+      <c r="Q13" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="15" t="s">
+      <c r="A14" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="5"/>
+      <c r="C14" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" s="29"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
@@ -1466,25 +1633,28 @@
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
+        <v>70</v>
+      </c>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
       <c r="M14" s="2"/>
       <c r="N14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="O14" s="9"/>
+      <c r="O14" s="8"/>
+      <c r="Q14" s="1"/>
     </row>
     <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="5"/>
+      <c r="C15" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="E15" s="29"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
@@ -1492,31 +1662,33 @@
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
+        <v>70</v>
+      </c>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
       <c r="M15" s="2"/>
       <c r="N15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="O15" s="9"/>
-      <c r="Q15" t="s">
-        <v>16</v>
+      <c r="O15" s="8"/>
+      <c r="Q15" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="5"/>
+      <c r="C16" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="E16" s="29"/>
       <c r="F16" s="2" t="s">
         <v>10</v>
       </c>
@@ -1526,24 +1698,26 @@
       <c r="J16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
       <c r="M16" s="2"/>
       <c r="N16" s="3"/>
-      <c r="O16" s="9"/>
-      <c r="Q16" t="s">
-        <v>18</v>
+      <c r="O16" s="8"/>
+      <c r="Q16" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="5"/>
+      <c r="C17" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="E17" s="29"/>
       <c r="F17" s="2" t="s">
         <v>10</v>
       </c>
@@ -1555,24 +1729,24 @@
       <c r="J17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
       <c r="M17" s="2"/>
       <c r="N17" s="3"/>
-      <c r="O17" s="9"/>
-      <c r="Q17" t="s">
-        <v>17</v>
-      </c>
+      <c r="O17" s="8"/>
+      <c r="Q17" s="1"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="5"/>
+      <c r="C18" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="E18" s="29"/>
       <c r="F18" s="2" t="s">
         <v>10</v>
       </c>
@@ -1584,21 +1758,26 @@
       <c r="J18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
       <c r="M18" s="2"/>
       <c r="N18" s="3"/>
-      <c r="O18" s="9"/>
+      <c r="O18" s="8"/>
+      <c r="Q18" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="5"/>
+      <c r="C19" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="E19" s="29"/>
       <c r="F19" s="2" t="s">
         <v>10</v>
       </c>
@@ -1610,24 +1789,26 @@
       <c r="J19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
       <c r="M19" s="2"/>
       <c r="N19" s="3"/>
-      <c r="O19" s="9"/>
-      <c r="Q19" t="s">
-        <v>62</v>
+      <c r="O19" s="8"/>
+      <c r="Q19" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="5"/>
+      <c r="C20" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="E20" s="29"/>
       <c r="F20" s="2" t="s">
         <v>10</v>
       </c>
@@ -1637,24 +1818,26 @@
       <c r="J20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
       <c r="M20" s="2"/>
       <c r="N20" s="3"/>
-      <c r="O20" s="9"/>
-      <c r="Q20" t="s">
-        <v>63</v>
+      <c r="O20" s="8"/>
+      <c r="Q20" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="5"/>
+      <c r="C21" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="E21" s="29"/>
       <c r="F21" s="2" t="s">
         <v>10</v>
       </c>
@@ -1666,21 +1849,24 @@
       <c r="J21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
       <c r="M21" s="2"/>
       <c r="N21" s="3"/>
-      <c r="O21" s="9"/>
+      <c r="O21" s="8"/>
+      <c r="Q21" s="1"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="5"/>
+      <c r="C22" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="E22" s="29"/>
       <c r="F22" s="2" t="s">
         <v>10</v>
       </c>
@@ -1692,21 +1878,26 @@
       <c r="J22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
       <c r="M22" s="2"/>
       <c r="N22" s="3"/>
-      <c r="O22" s="9"/>
+      <c r="O22" s="8"/>
+      <c r="Q22" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="5"/>
+      <c r="C23" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="E23" s="29"/>
       <c r="F23" s="2" t="s">
         <v>10</v>
       </c>
@@ -1718,24 +1909,29 @@
       <c r="J23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
       <c r="M23" s="2"/>
       <c r="N23" s="3"/>
-      <c r="O23" s="9"/>
+      <c r="O23" s="8"/>
+      <c r="Q23" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="5"/>
+      <c r="B24" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="E24" s="29"/>
       <c r="F24" s="2" t="s">
         <v>10</v>
       </c>
@@ -1747,23 +1943,25 @@
       <c r="J24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
       <c r="M24" s="2"/>
       <c r="N24" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="O24" s="9"/>
+      <c r="O24" s="8"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B25" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="5"/>
+      <c r="B25" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="E25" s="29"/>
       <c r="F25" s="2" t="s">
         <v>10</v>
       </c>
@@ -1775,23 +1973,25 @@
       <c r="J25" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
       <c r="M25" s="2"/>
       <c r="N25" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="O25" s="9"/>
+      <c r="O25" s="8"/>
     </row>
     <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="5"/>
+      <c r="B26" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="E26" s="29"/>
       <c r="F26" s="2" t="s">
         <v>10</v>
       </c>
@@ -1803,28 +2003,28 @@
       <c r="J26" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
       <c r="M26" s="2"/>
       <c r="N26" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="O26" s="9"/>
+      <c r="O26" s="8"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="D27" s="4" t="s">
+      <c r="A27" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D27" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="5"/>
+      <c r="E27" s="29"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -1832,21 +2032,23 @@
         <v>10</v>
       </c>
       <c r="J27" s="2"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
       <c r="M27" s="2"/>
       <c r="N27" s="3"/>
-      <c r="O27" s="9"/>
+      <c r="O27" s="8"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B28" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="5"/>
+      <c r="B28" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="29"/>
       <c r="F28" s="2" t="s">
         <v>10</v>
       </c>
@@ -1856,23 +2058,23 @@
       <c r="J28" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
       <c r="M28" s="2"/>
       <c r="N28" s="3"/>
-      <c r="O28" s="9"/>
+      <c r="O28" s="8"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B29" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C29" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="D29" s="4" t="s">
+      <c r="B29" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="E29" s="5"/>
+      <c r="E29" s="29"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -1880,23 +2082,25 @@
         <v>10</v>
       </c>
       <c r="J29" s="2"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
       <c r="M29" s="2"/>
       <c r="N29" s="3"/>
-      <c r="O29" s="9"/>
-      <c r="T29" s="12"/>
-      <c r="U29" s="12"/>
+      <c r="O29" s="8"/>
+      <c r="T29" s="11"/>
+      <c r="U29" s="11"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B30" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="5"/>
+      <c r="B30" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" s="29"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2" t="s">
         <v>10</v>
@@ -1906,23 +2110,23 @@
       <c r="J30" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
       <c r="M30" s="2"/>
       <c r="N30" s="3"/>
-      <c r="O30" s="9"/>
+      <c r="O30" s="8"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B31" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="D31" s="4" t="s">
+      <c r="B31" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D31" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="5"/>
+      <c r="E31" s="29"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -1930,21 +2134,23 @@
         <v>10</v>
       </c>
       <c r="J31" s="2"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
       <c r="M31" s="2"/>
       <c r="N31" s="3"/>
-      <c r="O31" s="9"/>
+      <c r="O31" s="8"/>
     </row>
     <row r="32" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C32" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="5"/>
+      <c r="B32" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="29"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2" t="s">
@@ -1954,28 +2160,28 @@
       <c r="J32" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
       <c r="M32" s="2"/>
       <c r="N32" s="3"/>
-      <c r="O32" s="9"/>
-      <c r="T32" s="12"/>
-      <c r="U32" s="12"/>
+      <c r="O32" s="8"/>
+      <c r="T32" s="11"/>
+      <c r="U32" s="11"/>
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="D33" s="4" t="s">
+      <c r="B33" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D33" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="E33" s="5"/>
+      <c r="E33" s="29"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -1983,23 +2189,25 @@
         <v>10</v>
       </c>
       <c r="J33" s="2"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
       <c r="M33" s="2"/>
       <c r="N33" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="O33" s="9"/>
+      <c r="O33" s="8"/>
     </row>
     <row r="34" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B34" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="5"/>
+      <c r="B34" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="E34" s="29"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -2007,23 +2215,25 @@
       <c r="J34" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
       <c r="M34" s="2" t="s">
         <v>10</v>
       </c>
       <c r="N34" s="3"/>
-      <c r="O34" s="9"/>
+      <c r="O34" s="8"/>
     </row>
     <row r="35" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B35" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="5"/>
+      <c r="B35" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="E35" s="29"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
@@ -2031,35 +2241,37 @@
       <c r="J35" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
       <c r="M35" s="2" t="s">
         <v>10</v>
       </c>
       <c r="N35" s="3"/>
-      <c r="O35" s="9"/>
-      <c r="W35" s="12"/>
-      <c r="X35" s="12"/>
-      <c r="Y35" s="12"/>
-      <c r="Z35" s="12"/>
-      <c r="AA35" s="12"/>
-      <c r="AB35" s="12"/>
-      <c r="AC35" s="12"/>
-      <c r="AD35" s="12"/>
-      <c r="AE35" s="12"/>
-      <c r="AF35" s="12"/>
-      <c r="AG35" s="12"/>
-      <c r="AH35" s="12"/>
+      <c r="O35" s="8"/>
+      <c r="W35" s="11"/>
+      <c r="X35" s="11"/>
+      <c r="Y35" s="11"/>
+      <c r="Z35" s="11"/>
+      <c r="AA35" s="11"/>
+      <c r="AB35" s="11"/>
+      <c r="AC35" s="11"/>
+      <c r="AD35" s="11"/>
+      <c r="AE35" s="11"/>
+      <c r="AF35" s="11"/>
+      <c r="AG35" s="11"/>
+      <c r="AH35" s="11"/>
     </row>
     <row r="36" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C36" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="5"/>
+      <c r="C36" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D36" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E36" s="29"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -2067,40 +2279,40 @@
       <c r="J36" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
       <c r="M36" s="2" t="s">
         <v>10</v>
       </c>
       <c r="N36" s="3"/>
-      <c r="O36" s="9"/>
-      <c r="W36" s="12"/>
-      <c r="X36" s="12"/>
-      <c r="Y36" s="12"/>
-      <c r="Z36" s="12"/>
-      <c r="AA36" s="12"/>
-      <c r="AB36" s="12"/>
-      <c r="AC36" s="12"/>
-      <c r="AD36" s="12"/>
-      <c r="AE36" s="12"/>
-      <c r="AF36" s="12"/>
-      <c r="AG36" s="12"/>
-      <c r="AH36" s="12"/>
+      <c r="O36" s="8"/>
+      <c r="W36" s="11"/>
+      <c r="X36" s="11"/>
+      <c r="Y36" s="11"/>
+      <c r="Z36" s="11"/>
+      <c r="AA36" s="11"/>
+      <c r="AB36" s="11"/>
+      <c r="AC36" s="11"/>
+      <c r="AD36" s="11"/>
+      <c r="AE36" s="11"/>
+      <c r="AF36" s="11"/>
+      <c r="AG36" s="11"/>
+      <c r="AH36" s="11"/>
     </row>
     <row r="37" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B37" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="C37" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E37" s="5"/>
+      <c r="B37" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="D37" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="E37" s="29"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
@@ -2108,196 +2320,188 @@
       <c r="J37" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
       <c r="M37" s="2"/>
       <c r="N37" s="3"/>
-      <c r="O37" s="9"/>
-      <c r="W37" s="12"/>
-      <c r="X37" s="12"/>
-      <c r="Y37" s="12"/>
-      <c r="Z37" s="12"/>
-      <c r="AA37" s="12"/>
-      <c r="AB37" s="12"/>
-      <c r="AC37" s="12"/>
-      <c r="AD37" s="12"/>
-      <c r="AE37" s="12"/>
-      <c r="AF37" s="12"/>
-      <c r="AG37" s="12"/>
-      <c r="AH37" s="12"/>
-    </row>
-    <row r="38" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C38" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E38" s="5"/>
+      <c r="O37" s="8"/>
+      <c r="W37" s="11"/>
+      <c r="X37" s="11"/>
+      <c r="Y37" s="11"/>
+      <c r="Z37" s="11"/>
+      <c r="AA37" s="11"/>
+      <c r="AB37" s="11"/>
+      <c r="AC37" s="11"/>
+      <c r="AD37" s="11"/>
+      <c r="AE37" s="11"/>
+      <c r="AF37" s="11"/>
+      <c r="AG37" s="11"/>
+      <c r="AH37" s="11"/>
+    </row>
+    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B38" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="E38" s="29"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
-      <c r="K38" s="5"/>
-      <c r="L38" s="5"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
       <c r="M38" s="2"/>
       <c r="N38" s="3"/>
-      <c r="O38" s="9"/>
-      <c r="W38" s="12"/>
-      <c r="X38" s="12"/>
-      <c r="Y38" s="12"/>
-      <c r="Z38" s="12"/>
-      <c r="AA38" s="12"/>
-      <c r="AB38" s="12"/>
-      <c r="AC38" s="12"/>
-      <c r="AD38" s="12"/>
-      <c r="AE38" s="12"/>
-      <c r="AF38" s="12"/>
-      <c r="AG38" s="12"/>
-      <c r="AH38" s="12"/>
-    </row>
-    <row r="39" spans="1:34" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="24" t="s">
+      <c r="O38" s="8"/>
+      <c r="W38" s="11"/>
+      <c r="X38" s="11"/>
+      <c r="Y38" s="11"/>
+      <c r="Z38" s="11"/>
+      <c r="AA38" s="11"/>
+      <c r="AB38" s="11"/>
+      <c r="AC38" s="11"/>
+      <c r="AD38" s="11"/>
+      <c r="AE38" s="11"/>
+      <c r="AF38" s="11"/>
+      <c r="AG38" s="11"/>
+      <c r="AH38" s="11"/>
+    </row>
+    <row r="39" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B39" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="D39" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="E39" s="29"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="8"/>
+      <c r="W39" s="11"/>
+      <c r="X39" s="11"/>
+      <c r="Y39" s="11"/>
+      <c r="Z39" s="11"/>
+      <c r="AA39" s="11"/>
+      <c r="AB39" s="11"/>
+      <c r="AC39" s="11"/>
+      <c r="AD39" s="11"/>
+      <c r="AE39" s="11"/>
+      <c r="AF39" s="11"/>
+      <c r="AG39" s="11"/>
+    </row>
+    <row r="40" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="B39" s="25"/>
-      <c r="C39" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E39" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F39" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="G39" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="H39" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="I39" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="J39" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="K39" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="L39" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="M39" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="N39" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="O39" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="W39" s="12"/>
-      <c r="X39" s="12"/>
-      <c r="Y39" s="12"/>
-      <c r="Z39" s="12"/>
-      <c r="AA39" s="12"/>
-      <c r="AB39" s="12"/>
-      <c r="AC39" s="12"/>
-      <c r="AD39" s="12"/>
-      <c r="AE39" s="12"/>
-      <c r="AF39" s="12"/>
-      <c r="AG39" s="12"/>
-    </row>
-    <row r="40" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B40" s="31" t="s">
-        <v>124</v>
-      </c>
-      <c r="C40" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="D40" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
+      <c r="D40" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="E40" s="29"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
       <c r="I40" s="2"/>
-      <c r="J40" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
       <c r="M40" s="2"/>
       <c r="N40" s="3"/>
-      <c r="O40" s="28"/>
-      <c r="W40" s="12"/>
-      <c r="X40" s="12"/>
-      <c r="Y40" s="12"/>
-      <c r="Z40" s="12"/>
-      <c r="AA40" s="12"/>
-      <c r="AB40" s="12"/>
-      <c r="AC40" s="12"/>
-      <c r="AD40" s="12"/>
-      <c r="AE40" s="12"/>
-      <c r="AF40" s="12"/>
-      <c r="AG40" s="12"/>
-    </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A41" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="B41" s="32" t="s">
+      <c r="O40" s="8"/>
+      <c r="W40" s="11"/>
+      <c r="X40" s="11"/>
+      <c r="Y40" s="11"/>
+      <c r="Z40" s="11"/>
+      <c r="AA40" s="11"/>
+      <c r="AB40" s="11"/>
+      <c r="AC40" s="11"/>
+      <c r="AD40" s="11"/>
+      <c r="AE40" s="11"/>
+      <c r="AF40" s="11"/>
+      <c r="AG40" s="11"/>
+    </row>
+    <row r="41" spans="1:34" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="B41" s="38"/>
+      <c r="C41" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E41" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F41" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H41" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="I41" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="J41" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="K41" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="L41" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="M41" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="N41" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="O41" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="T41" s="11"/>
+      <c r="U41" s="11"/>
+    </row>
+    <row r="42" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="D42" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="C41" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="D41" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="E41" s="2"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="3"/>
-      <c r="O41" s="28"/>
-      <c r="T41" s="12"/>
-      <c r="U41" s="12"/>
-    </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="C42" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="D42" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="E42" s="2"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2" t="s">
         <v>10</v>
@@ -2306,35 +2510,110 @@
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="3"/>
-      <c r="O42" s="28"/>
+      <c r="O42" s="3"/>
+    </row>
+    <row r="43" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="D43" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="E43" s="30"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+    </row>
+    <row r="44" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A44" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B44" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="D44" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="E44" s="30"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="3"/>
+      <c r="O44" s="3"/>
     </row>
     <row r="45" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="T45" s="12"/>
-      <c r="U45" s="12"/>
+      <c r="A45" s="1"/>
+      <c r="B45" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="D45" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="E45" s="30"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="3"/>
+      <c r="O45" s="3"/>
+      <c r="T45" s="11"/>
+      <c r="U45" s="11"/>
     </row>
     <row r="50" spans="20:21" x14ac:dyDescent="0.25">
-      <c r="T50" s="12"/>
-      <c r="U50" s="12"/>
+      <c r="T50" s="11"/>
+      <c r="U50" s="11"/>
     </row>
     <row r="55" spans="20:21" x14ac:dyDescent="0.25">
-      <c r="T55" s="12"/>
-      <c r="U55" s="12"/>
+      <c r="T55" s="11"/>
+      <c r="U55" s="11"/>
     </row>
     <row r="72" spans="16:23" x14ac:dyDescent="0.25">
-      <c r="P72" s="12"/>
-      <c r="Q72" s="12"/>
-      <c r="R72" s="12"/>
-      <c r="S72" s="12"/>
-      <c r="T72" s="12"/>
-      <c r="U72" s="12"/>
-      <c r="V72" s="12"/>
-      <c r="W72" s="12"/>
+      <c r="P72" s="11"/>
+      <c r="Q72" s="11"/>
+      <c r="R72" s="11"/>
+      <c r="S72" s="11"/>
+      <c r="T72" s="11"/>
+      <c r="U72" s="11"/>
+      <c r="V72" s="11"/>
+      <c r="W72" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A41:B41"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2357,72 +2636,72 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="27"/>
+      <c r="A2" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="40"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="27"/>
+      <c r="A13" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="40"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>